<commit_message>
docs updated. background images updated
</commit_message>
<xml_diff>
--- a/DesignDocs/BackgroundConcepts.xlsx
+++ b/DesignDocs/BackgroundConcepts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\Unity 2D\GreatGame\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF58816-9D43-4CE6-8FAC-D91F84EA45E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2CE2E6-B48C-403E-9434-40C8121BE58C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7110" yWindow="2475" windowWidth="21600" windowHeight="11385" xr2:uid="{5238B777-0F4E-44C7-BC99-EEF756CA3825}"/>
+    <workbookView xWindow="33405" yWindow="2610" windowWidth="21600" windowHeight="11385" xr2:uid="{5238B777-0F4E-44C7-BC99-EEF756CA3825}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -621,14 +621,14 @@
   <dimension ref="B2:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="82.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
@@ -687,7 +687,7 @@
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -698,7 +698,7 @@
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -709,7 +709,7 @@
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -720,7 +720,7 @@
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -731,7 +731,7 @@
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -742,7 +742,7 @@
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -753,7 +753,7 @@
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="1" t="s">

</xml_diff>